<commit_message>
Added new test class to test ones. Updated Test Oracle with new findings Refactored
</commit_message>
<xml_diff>
--- a/BusArrivalEstimaterTest/TestOracle.xlsx
+++ b/BusArrivalEstimaterTest/TestOracle.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\Visual Studio 2015\Projects\BusArrivalEstimater\BusArrivalEstimaterTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\visual studio 2015\Projects\BusArrivalEstimater\BusArrivalEstimaterTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -44,17 +46,56 @@
     <t>Total Bus Per Min</t>
   </si>
   <si>
-    <t>Average Wait Time For A Bus</t>
-  </si>
-  <si>
     <t>Max Wait Time For A Bus</t>
+  </si>
+  <si>
+    <t>1 1</t>
+  </si>
+  <si>
+    <t>1 1 1</t>
+  </si>
+  <si>
+    <t>1 1 1 1</t>
+  </si>
+  <si>
+    <t>2 2</t>
+  </si>
+  <si>
+    <t>2 2 2</t>
+  </si>
+  <si>
+    <t>2 2 2 2</t>
+  </si>
+  <si>
+    <t>1 1 1 1 1</t>
+  </si>
+  <si>
+    <t>(3/4)</t>
+  </si>
+  <si>
+    <t>(2/3)</t>
+  </si>
+  <si>
+    <t>(3/5)</t>
+  </si>
+  <si>
+    <t>(5/8)</t>
+  </si>
+  <si>
+    <t>Bus Freq</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +103,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,13 +165,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,23 +490,361 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>1/PRODUCT(B2:K2)</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.1666667</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.16666700000000001</v>
+      </c>
+      <c r="H8">
+        <f>C8/B8</f>
+        <v>0.75000075000075006</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:J8" si="0">D8/C8</f>
+        <v>0.8</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.83333500000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <f>B7/B8</f>
+        <v>0.75000075000075006</v>
+      </c>
+      <c r="C9" s="4">
+        <f>C7/C8</f>
+        <v>0.6666668</v>
+      </c>
+      <c r="D9" s="4">
+        <f>D7/D8</f>
+        <v>0.625</v>
+      </c>
+      <c r="E9" s="4">
+        <f>E7/E8</f>
+        <v>0.59999880000240002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <f>B13/B14</f>
+        <v>0.74999962500018746</v>
+      </c>
+      <c r="C15" s="2">
+        <f>C13/C14</f>
+        <v>0.66666599999999998</v>
+      </c>
+      <c r="D15" s="2">
+        <f>D13/D14</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.5</v>
+      </c>
+      <c r="B17">
+        <f>A17*B18/B19</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:G17" si="1">B17*C18/C19</f>
+        <v>0.25</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B2:H2)</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <f>COUNT(B2:H2)</f>
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>PRODUCT(B2:J2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>1/PRODUCT(B2:J2)</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>(SUM(B2:J2)*B2^2)/2</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>COUNT(B2:L2)/3*B2^3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>B11*(C11-D11)</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <f>IFERROR(1/B2,0)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:J3" si="0">IFERROR(1/C2,0)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -439,31 +875,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <f>SUM(B3:J3)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <f>SUM(B3:B3)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <f>1/B4</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <f>B5/2</f>
-        <v>0.25</v>
+        <f>1/B4/2</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>IF(C2,(B5*COUNT($B$2:C2)/(COUNT($B$2:C2)+1)),FALSE)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D5" t="b">
+        <f>IF(D2,(C5*COUNT($B$2:D2)/(COUNT($B$2:D2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <f>IF(E2,(D5*COUNT($B$2:E2)/(COUNT($B$2:E2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <f>IF(F2,(E5*COUNT($B$2:F2)/(COUNT($B$2:F2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <f>IF(G2,(F5*COUNT($B$2:G2)/(COUNT($B$2:G2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <f>IF(H2,(G5*COUNT($B$2:H2)/(COUNT($B$2:H2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <f>IF(I2,(H5*COUNT($B$2:I2)/(COUNT($B$2:I2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <f>IF(J2,(I5*COUNT($B$2:J2)/(COUNT($B$2:J2)+1)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <f>IF(K2,(J5*COUNT($B$2:K2)/(COUNT($B$2:K2)+1)),FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>